<commit_message>
thêm thư mục pojo, chỉnh sửa tài liệu
</commit_message>
<xml_diff>
--- a/SD.xlsx
+++ b/SD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Hoctap\LapTrinhUngDungJava\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Hoctap\LapTrinhUngDungJava\Project\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BB8BFD-A070-4D71-AB1B-650C72B7CABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07188A1-538A-4969-8201-CEFBF8DD58A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>1.</t>
   </si>
@@ -98,6 +98,78 @@
   </si>
   <si>
     <t>2. đăng ký phúc khảo điểm</t>
+  </si>
+  <si>
+    <t>SINH_VIEN</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>gioi_tinh</t>
+  </si>
+  <si>
+    <t>cmnd</t>
+  </si>
+  <si>
+    <t>TAI_KHOAN</t>
+  </si>
+  <si>
+    <t>mat_khau</t>
+  </si>
+  <si>
+    <t>liscen_id</t>
+  </si>
+  <si>
+    <t>SINH_VIEN_LOP</t>
+  </si>
+  <si>
+    <t>ma_sinh_vien</t>
+  </si>
+  <si>
+    <t>ma_lop</t>
+  </si>
+  <si>
+    <t>LOP</t>
+  </si>
+  <si>
+    <t>phong_hoc</t>
+  </si>
+  <si>
+    <t>MON_HOC</t>
+  </si>
+  <si>
+    <t>ngay_hoc</t>
+  </si>
+  <si>
+    <t>tiet_bat_dau</t>
+  </si>
+  <si>
+    <t>tiet_ket_thuc</t>
+  </si>
+  <si>
+    <t>LOP_MON_HOC</t>
+  </si>
+  <si>
+    <t>ma_mon_hoc</t>
+  </si>
+  <si>
+    <t>trang_thai_sinh_vien</t>
+  </si>
+  <si>
+    <t>diem_GK</t>
+  </si>
+  <si>
+    <t>diem_CK</t>
+  </si>
+  <si>
+    <t>diem_khac</t>
+  </si>
+  <si>
+    <t>diem_tong</t>
   </si>
 </sst>
 </file>
@@ -113,12 +185,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,9 +211,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,39 +581,39 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
         <v>19</v>
       </c>
     </row>
@@ -545,14 +624,148 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A776E66-7E3A-43B2-AA51-BDE0548DA0F8}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>